<commit_message>
Bernard Ong - latest test results.
</commit_message>
<xml_diff>
--- a/Algo-Results.xlsx
+++ b/Algo-Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\nycdsa-kaggle-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\nycdsa\Projects\04-Kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -52,16 +52,77 @@
   </si>
   <si>
     <t>Mean AMS Score</t>
+  </si>
+  <si>
+    <t>Bernard</t>
+  </si>
+  <si>
+    <t>Top Private Leaderboard Scores Benchmark</t>
+  </si>
+  <si>
+    <t>10 - 3.75838</t>
+  </si>
+  <si>
+    <t>15 - 3.74604</t>
+  </si>
+  <si>
+    <t>20 - 3.73932</t>
+  </si>
+  <si>
+    <t>30 - 3.72654</t>
+  </si>
+  <si>
+    <t>50 - 3.71768</t>
+  </si>
+  <si>
+    <t>3   - 3.78682</t>
+  </si>
+  <si>
+    <t>2   - 3.78913</t>
+  </si>
+  <si>
+    <t>1   - 3.80581</t>
+  </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>zeros</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Boosting</t>
+  </si>
+  <si>
+    <t>Best Combo So Far</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,8 +138,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +171,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -144,8 +233,44 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,49 +552,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="19" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14" style="8" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="10" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="11.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H11" s="19" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4">
+        <v>30</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.99202000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4">
+        <v>30</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0.97607999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="18">
+        <v>1.00702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4">
+        <v>30</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="20">
+        <v>1.00969</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="18">
+        <v>1.0027999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0.77995999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4">
+        <v>30</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="21">
+        <v>1.00983</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4">
+        <v>30</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0.88221000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="18">
+        <v>0.92456000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4">
+        <v>30</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0.83</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="18">
+        <v>1.7829900000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4">
+        <v>30</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="18">
+        <v>1.76413</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="4">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="18">
+        <v>1.55776</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4">
+        <v>30</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="21">
+        <v>1.8181499999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="4">
+        <v>30</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="18">
+        <v>1.7602599999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="4">
+        <v>30</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="18">
+        <v>3.5075699999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="4">
+        <v>30</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="18">
+        <v>3.5078999999999998</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nanda - test results for Boosting.
</commit_message>
<xml_diff>
--- a/Algo-Results.xlsx
+++ b/Algo-Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\nycdsa\Projects\04-Kaggle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Projects\04-Kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Tester</t>
+  </si>
+  <si>
+    <t>Nanda</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,8 +1067,86 @@
       <c r="H27" s="18">
         <v>3.5078999999999998</v>
       </c>
-      <c r="I27" s="22" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="4">
+        <v>30</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="18">
+        <v>3.5350000000000001</v>
+      </c>
+      <c r="I28" s="22" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="4">
+        <v>30</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="18">
+        <v>3.2513000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nanda - added new status for Boosting results.
</commit_message>
<xml_diff>
--- a/Algo-Results.xlsx
+++ b/Algo-Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Projects\04-Kaggle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\nycdsa-kaggle-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Nanda</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1142,8 @@
       <c r="G30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>30</v>
+      <c r="H30" s="18">
+        <v>3.5203000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest results file updated.
</commit_message>
<xml_diff>
--- a/Algo-Results.xlsx
+++ b/Algo-Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\nycdsa-kaggle-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Projects\04-Kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Threshold</t>
   </si>
   <si>
-    <t>Imputter</t>
-  </si>
-  <si>
     <t>Standardized</t>
   </si>
   <si>
@@ -115,6 +112,18 @@
   </si>
   <si>
     <t>Nanda</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>most_frequent</t>
+  </si>
+  <si>
+    <t>Imputer</t>
+  </si>
+  <si>
+    <t>Xval Folds</t>
   </si>
 </sst>
 </file>
@@ -164,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +189,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -273,6 +288,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -555,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,65 +600,66 @@
     <col min="2" max="2" width="19" style="12" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="18" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="11.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="18" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>1</v>
@@ -637,24 +671,27 @@
         <v>3</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4">
         <v>30</v>
@@ -663,24 +700,27 @@
         <v>0.85</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>19</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="18">
+        <v>19</v>
+      </c>
+      <c r="H12" s="27">
+        <v>3</v>
+      </c>
+      <c r="I12" s="18">
         <v>0.99202000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
         <v>30</v>
@@ -689,24 +729,27 @@
         <v>0.86</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="18">
+        <v>19</v>
+      </c>
+      <c r="H13" s="27">
+        <v>3</v>
+      </c>
+      <c r="I13" s="18">
         <v>0.97607999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4">
         <v>30</v>
@@ -715,24 +758,27 @@
         <v>0.84</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="18">
+        <v>19</v>
+      </c>
+      <c r="H14" s="27">
+        <v>3</v>
+      </c>
+      <c r="I14" s="18">
         <v>1.00702</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4">
         <v>30</v>
@@ -741,24 +787,27 @@
         <v>0.83</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="20">
+        <v>19</v>
+      </c>
+      <c r="H15" s="27">
+        <v>3</v>
+      </c>
+      <c r="I15" s="20">
         <v>1.00969</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="4">
         <v>30</v>
@@ -767,50 +816,56 @@
         <v>0.82</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="18">
+        <v>19</v>
+      </c>
+      <c r="H16" s="27">
+        <v>3</v>
+      </c>
+      <c r="I16" s="18">
         <v>1.0027999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4">
         <v>30</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="24">
         <v>0.83</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="18">
+      <c r="F17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="27">
+        <v>3</v>
+      </c>
+      <c r="I17" s="18">
         <v>0.77995999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="4">
         <v>30</v>
@@ -819,50 +874,56 @@
         <v>0.83</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="21">
+        <v>19</v>
+      </c>
+      <c r="H18" s="27">
+        <v>3</v>
+      </c>
+      <c r="I18" s="21">
         <v>1.00983</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4">
         <v>30</v>
       </c>
       <c r="D19" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="8" t="s">
+        <v>0.85</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>21</v>
       </c>
+      <c r="F19" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="G19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0.88221000000000005</v>
+        <v>19</v>
+      </c>
+      <c r="H19" s="27">
+        <v>3</v>
+      </c>
+      <c r="I19" s="18">
+        <v>0.99226999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4">
         <v>30</v>
@@ -871,50 +932,56 @@
         <v>0.83</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0.92456000000000005</v>
+        <v>19</v>
+      </c>
+      <c r="H20" s="27">
+        <v>3</v>
+      </c>
+      <c r="I20" s="18">
+        <v>0.88221000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4">
         <v>30</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="6">
         <v>0.83</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="18">
-        <v>1.7829900000000001</v>
+        <v>23</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="27">
+        <v>3</v>
+      </c>
+      <c r="I21" s="18">
+        <v>0.92456000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4">
         <v>30</v>
@@ -922,25 +989,28 @@
       <c r="D22" s="6">
         <v>0.83</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>22</v>
+      <c r="E22" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="18">
-        <v>1.76413</v>
+        <v>19</v>
+      </c>
+      <c r="H22" s="27">
+        <v>3</v>
+      </c>
+      <c r="I22" s="26">
+        <v>0.91496</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4">
         <v>30</v>
@@ -949,50 +1019,56 @@
         <v>0.83</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="18">
-        <v>1.55776</v>
+        <v>19</v>
+      </c>
+      <c r="H23" s="27">
+        <v>3</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0.88797999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="4">
         <v>30</v>
       </c>
-      <c r="D24" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="D24" s="17">
+        <v>0.83</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="21">
-        <v>1.8181499999999999</v>
+      <c r="F24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="27">
+        <v>3</v>
+      </c>
+      <c r="I24" s="18">
+        <v>1.7829900000000001</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4">
         <v>30</v>
@@ -1001,24 +1077,27 @@
         <v>0.83</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="18">
-        <v>1.7602599999999999</v>
+        <v>19</v>
+      </c>
+      <c r="H25" s="27">
+        <v>3</v>
+      </c>
+      <c r="I25" s="18">
+        <v>1.76413</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4">
         <v>30</v>
@@ -1027,24 +1106,27 @@
         <v>0.83</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="18">
-        <v>3.5075699999999999</v>
+      <c r="H26" s="27">
+        <v>3</v>
+      </c>
+      <c r="I26" s="18">
+        <v>1.55776</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" s="4">
         <v>30</v>
@@ -1052,98 +1134,458 @@
       <c r="D27" s="6">
         <v>0.83</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="E27" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="18">
-        <v>3.5078999999999998</v>
+        <v>19</v>
+      </c>
+      <c r="H27" s="27">
+        <v>3</v>
+      </c>
+      <c r="I27" s="20">
+        <v>1.8181499999999999</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4">
         <v>30</v>
       </c>
       <c r="D28" s="6">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="18">
-        <v>3.5350000000000001</v>
-      </c>
-      <c r="I28" s="22" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="H28" s="27">
+        <v>3</v>
+      </c>
+      <c r="I28" s="18">
+        <v>1.7602599999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="4">
+        <v>30</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="4">
-        <v>30</v>
-      </c>
-      <c r="D29" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="F29" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="18">
-        <v>3.2513000000000001</v>
+        <v>19</v>
+      </c>
+      <c r="H29" s="27">
+        <v>3</v>
+      </c>
+      <c r="I29" s="18">
+        <v>1.78949</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="4">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="27">
+        <v>3</v>
+      </c>
+      <c r="I30" s="21">
+        <v>1.8185199999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4">
+        <v>30</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="27">
+        <v>3</v>
+      </c>
+      <c r="I31" s="18">
+        <v>3.5075699999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="4">
+        <v>30</v>
+      </c>
+      <c r="D32" s="24">
+        <v>0.83</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="27">
+        <v>3</v>
+      </c>
+      <c r="I32" s="18">
+        <v>3.5078999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="4">
+        <v>30</v>
+      </c>
+      <c r="D33" s="17">
+        <v>0.85</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="27">
+        <v>3</v>
+      </c>
+      <c r="I33" s="28">
+        <v>3.5350000000000001</v>
+      </c>
+      <c r="J33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="4">
-        <v>30</v>
-      </c>
-      <c r="D30" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="E30" s="8" t="s">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="4">
+        <v>30</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="27">
+        <v>3</v>
+      </c>
+      <c r="I34" s="18">
+        <v>3.2513000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="4">
+        <v>30</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="27">
+        <v>3</v>
+      </c>
+      <c r="I35" s="18">
+        <v>3.5203000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="4">
+        <v>30</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="27">
+        <v>3</v>
+      </c>
+      <c r="I36" s="18">
+        <v>3.5076000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="4">
+        <v>30</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="27">
+        <v>3</v>
+      </c>
+      <c r="I37" s="26">
+        <v>3.5293000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="4">
+        <v>30</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E38" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="18">
-        <v>3.5203000000000002</v>
+      <c r="F38" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="27">
+        <v>3</v>
+      </c>
+      <c r="I38" s="26">
+        <v>3.5200999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="4">
+        <v>30</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="27">
+        <v>3</v>
+      </c>
+      <c r="I39" s="18">
+        <v>3.5341999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="4">
+        <v>30</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="27">
+        <v>3</v>
+      </c>
+      <c r="I40" s="18">
+        <v>3.4964</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="4">
+        <v>30</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="27">
+        <v>3</v>
+      </c>
+      <c r="I41" s="18">
+        <v>3.5078999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="4">
+        <v>30</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="27">
+        <v>3</v>
+      </c>
+      <c r="I42" s="18">
+        <v>3.5224199999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>